<commit_message>
added in recommendations for water quality
</commit_message>
<xml_diff>
--- a/shinyApp/data/recommendations.xlsx
+++ b/shinyApp/data/recommendations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/DSPG_Floyd/shinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C887B0E4-6EAD-914E-A98C-C4BBAD9DAEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F26BBA-3288-7042-BFA7-805DA32E4871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="28800" windowHeight="16440" xr2:uid="{ACE92E2C-646A-E04C-93BC-CE46D57E8DD7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Manganese </t>
   </si>
@@ -54,9 +54,6 @@
     <t xml:space="preserve">Issue </t>
   </si>
   <si>
-    <t xml:space="preserve">Solution </t>
-  </si>
-  <si>
     <t xml:space="preserve">cation exchange water softening, distillation, filtration, and reverse osmosis </t>
   </si>
   <si>
@@ -70,13 +67,22 @@
   </si>
   <si>
     <t xml:space="preserve">Let water run until temperature, only use cold water </t>
+  </si>
+  <si>
+    <t>Reommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardness </t>
+  </si>
+  <si>
+    <t>commonly softened by using a tank containing an ion-exchange material, which takes up the calcium, magnesium and small amounts of dissolved iron from water in exchange for sodium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,15 +92,20 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -122,13 +133,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -445,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5B69A5-1C10-864B-AC65-50D7D0F46EC8}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -453,56 +464,64 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="38" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
+    <row r="7" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
republished, changes data to csv files
</commit_message>
<xml_diff>
--- a/shinyApp/data/recommendations.xlsx
+++ b/shinyApp/data/recommendations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/DSPG_Floyd/shinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F26BBA-3288-7042-BFA7-805DA32E4871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADA4FF1-7F6E-5248-B98D-435791A8AFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="28800" windowHeight="16440" xr2:uid="{ACE92E2C-646A-E04C-93BC-CE46D57E8DD7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Manganese </t>
   </si>
@@ -54,6 +54,9 @@
     <t xml:space="preserve">Issue </t>
   </si>
   <si>
+    <t xml:space="preserve">Solution </t>
+  </si>
+  <si>
     <t xml:space="preserve">cation exchange water softening, distillation, filtration, and reverse osmosis </t>
   </si>
   <si>
@@ -67,22 +70,13 @@
   </si>
   <si>
     <t xml:space="preserve">Let water run until temperature, only use cold water </t>
-  </si>
-  <si>
-    <t>Reommendation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardness </t>
-  </si>
-  <si>
-    <t>commonly softened by using a tank containing an ion-exchange material, which takes up the calcium, magnesium and small amounts of dissolved iron from water in exchange for sodium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,20 +86,15 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -133,13 +122,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -456,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5B69A5-1C10-864B-AC65-50D7D0F46EC8}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -464,64 +453,56 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="38" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>